<commit_message>
cleaned up old graphs and made new ones
</commit_message>
<xml_diff>
--- a/Iter1-analysisPairs.xlsx
+++ b/Iter1-analysisPairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheoryDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321F8B1A-2170-495C-BCCA-2A55DA045533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A621C742-8699-40B2-B1E1-4A4AE92B6D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="1802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3374" uniqueCount="1802">
   <si>
     <t>UID</t>
   </si>
@@ -5828,8 +5828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S81" sqref="S81"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB98" sqref="AB98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5930,7 +5930,7 @@
       </c>
       <c r="AD2">
         <f>COUNTIF(S2:S101,AC2)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -5965,17 +5965,17 @@
         <v>13</v>
       </c>
       <c r="S3" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Z3">
         <v>2</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA34" si="0">AA2+(IF(ISNUMBER(S3),1,0))</f>
+        <f>AA2+IF(S3 &gt; 0,1,0)</f>
         <v>2</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB66" si="1">AA3/Z3</f>
+        <f t="shared" ref="AB3:AB66" si="0">AA3/Z3</f>
         <v>1</v>
       </c>
       <c r="AC3">
@@ -5983,7 +5983,7 @@
       </c>
       <c r="AD3">
         <f>COUNTIF(S2:S101,AC3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
@@ -6024,11 +6024,11 @@
         <v>3</v>
       </c>
       <c r="AA4">
+        <f>AA3+IF(S4 &gt; 0,1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="AB4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AB4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC4">
@@ -6036,7 +6036,7 @@
       </c>
       <c r="AD4">
         <f>COUNTIF(S2:S101,AC4)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
@@ -6071,25 +6071,25 @@
         <v>17</v>
       </c>
       <c r="S5" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z5">
         <v>4</v>
       </c>
       <c r="AA5">
+        <f t="shared" ref="AA5:AA68" si="1">AA4+IF(S5 &gt; 0,1,0)</f>
+        <v>3</v>
+      </c>
+      <c r="AB5">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AC5">
         <v>4</v>
       </c>
       <c r="AD5">
         <f>COUNTIF(S2:S101,AC5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
@@ -6130,19 +6130,19 @@
         <v>5</v>
       </c>
       <c r="AA6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC6">
         <v>6</v>
       </c>
       <c r="AD6">
         <f>COUNTIF(S2:S101,AC6)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
@@ -6177,25 +6177,25 @@
         <v>21</v>
       </c>
       <c r="S7" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Z7">
         <v>6</v>
       </c>
       <c r="AA7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AB7">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="AB7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="AC7">
         <v>7</v>
       </c>
       <c r="AD7">
         <f>COUNTIF(S2:S101,AC7)</f>
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
@@ -6230,25 +6230,25 @@
         <v>23</v>
       </c>
       <c r="S8" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Z8">
         <v>7</v>
       </c>
       <c r="AA8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AB8">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="AC8">
         <v>8</v>
       </c>
       <c r="AD8">
         <f>COUNTIF(S2:S101,AC8)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
@@ -6283,25 +6283,25 @@
         <v>25</v>
       </c>
       <c r="S9" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z9">
         <v>8</v>
       </c>
       <c r="AA9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="AC9">
         <v>9</v>
       </c>
       <c r="AD9">
         <f>COUNTIF(S2:S101,AC9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
@@ -6335,18 +6335,18 @@
       <c r="Q10" t="s">
         <v>27</v>
       </c>
-      <c r="S10" s="3" t="s">
-        <v>715</v>
+      <c r="S10" s="3">
+        <v>7</v>
       </c>
       <c r="Z10">
         <v>9</v>
       </c>
       <c r="AA10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="AC10">
@@ -6388,19 +6388,19 @@
       <c r="Q11" t="s">
         <v>27</v>
       </c>
-      <c r="S11" s="3" t="s">
-        <v>715</v>
+      <c r="S11" s="3">
+        <v>7</v>
       </c>
       <c r="Z11">
         <v>10</v>
       </c>
       <c r="AA11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AB11">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="AC11">
         <v>12</v>
@@ -6442,25 +6442,25 @@
         <v>30</v>
       </c>
       <c r="S12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z12">
         <v>11</v>
       </c>
       <c r="AA12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="1"/>
-        <v>0.81818181818181823</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="AC12">
         <v>13</v>
       </c>
       <c r="AD12">
         <f>COUNTIF(S2:S101,AC12)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
@@ -6495,18 +6495,18 @@
         <v>32</v>
       </c>
       <c r="S13" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z13">
         <v>12</v>
       </c>
       <c r="AA13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="AC13">
         <v>14</v>
@@ -6548,18 +6548,18 @@
         <v>34</v>
       </c>
       <c r="S14" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z14">
         <v>13</v>
       </c>
       <c r="AA14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AB14">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="1"/>
-        <v>0.84615384615384615</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="AC14">
         <v>15</v>
@@ -6601,18 +6601,18 @@
         <v>36</v>
       </c>
       <c r="S15" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Z15">
         <v>14</v>
       </c>
       <c r="AA15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AB15">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="AB15">
-        <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AC15">
         <v>16</v>
@@ -6660,12 +6660,12 @@
         <v>15</v>
       </c>
       <c r="AA16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AB16">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="AB16">
-        <f t="shared" si="1"/>
-        <v>0.8666666666666667</v>
+        <v>0.93333333333333335</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
@@ -6700,18 +6700,18 @@
         <v>38</v>
       </c>
       <c r="S17" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z17">
         <v>16</v>
       </c>
       <c r="AA17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="AB17">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="AB17">
-        <f t="shared" si="1"/>
-        <v>0.875</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
@@ -6746,17 +6746,17 @@
         <v>40</v>
       </c>
       <c r="S18" s="1">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="Z18">
         <v>17</v>
       </c>
       <c r="AA18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="1"/>
         <v>0.88235294117647056</v>
       </c>
     </row>
@@ -6792,17 +6792,17 @@
         <v>42</v>
       </c>
       <c r="S19" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Z19">
         <v>18</v>
       </c>
       <c r="AA19">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AB19">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -6838,18 +6838,18 @@
         <v>399</v>
       </c>
       <c r="S20" s="1">
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="Z20">
         <v>19</v>
       </c>
       <c r="AA20">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AB20">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB20">
-        <f t="shared" si="1"/>
-        <v>0.89473684210526316</v>
+        <v>0.84210526315789469</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
@@ -6884,18 +6884,18 @@
         <v>779</v>
       </c>
       <c r="S21" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z21">
         <v>20</v>
       </c>
       <c r="AA21">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
@@ -6930,18 +6930,18 @@
         <v>44</v>
       </c>
       <c r="S22" s="1">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z22">
         <v>21</v>
       </c>
       <c r="AA22">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="AB22">
-        <f t="shared" si="1"/>
-        <v>0.90476190476190477</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
@@ -6976,18 +6976,18 @@
         <v>46</v>
       </c>
       <c r="S23" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z23">
         <v>22</v>
       </c>
       <c r="AA23">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="AB23">
-        <f t="shared" si="1"/>
-        <v>0.90909090909090906</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
@@ -7022,18 +7022,18 @@
         <v>48</v>
       </c>
       <c r="S24" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z24">
         <v>23</v>
       </c>
       <c r="AA24">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="AB24">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="AB24">
-        <f t="shared" si="1"/>
-        <v>0.91304347826086951</v>
+        <v>0.82608695652173914</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
@@ -7068,7 +7068,7 @@
         <v>44</v>
       </c>
       <c r="S25" s="4">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="U25" t="s">
         <v>1760</v>
@@ -7077,12 +7077,12 @@
         <v>24</v>
       </c>
       <c r="AA25">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="AB25">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="AB25">
-        <f t="shared" si="1"/>
-        <v>0.91666666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
@@ -7116,8 +7116,8 @@
       <c r="Q26" t="s">
         <v>51</v>
       </c>
-      <c r="S26" s="5" t="s">
-        <v>716</v>
+      <c r="S26" s="5">
+        <v>7</v>
       </c>
       <c r="U26" t="s">
         <v>717</v>
@@ -7129,12 +7129,12 @@
         <v>25</v>
       </c>
       <c r="AA26">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="1"/>
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
@@ -7169,18 +7169,18 @@
         <v>53</v>
       </c>
       <c r="S27" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z27">
         <v>26</v>
       </c>
       <c r="AA27">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="AB27">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="AB27">
-        <f t="shared" si="1"/>
-        <v>0.88461538461538458</v>
+        <v>0.80769230769230771</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
@@ -7214,19 +7214,19 @@
       <c r="Q28" t="s">
         <v>55</v>
       </c>
-      <c r="S28" s="3" t="s">
-        <v>715</v>
+      <c r="S28" s="3">
+        <v>7</v>
       </c>
       <c r="Z28">
         <v>27</v>
       </c>
       <c r="AA28">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="AB28">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="AB28">
-        <f t="shared" si="1"/>
-        <v>0.85185185185185186</v>
+        <v>0.81481481481481477</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
@@ -7261,18 +7261,18 @@
         <v>57</v>
       </c>
       <c r="S29" s="1">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="Z29">
         <v>28</v>
       </c>
       <c r="AA29">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="AB29">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="AB29">
-        <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
@@ -7306,19 +7306,19 @@
       <c r="Q30" t="s">
         <v>70</v>
       </c>
-      <c r="S30" s="5" t="s">
-        <v>716</v>
+      <c r="S30" s="5">
+        <v>6</v>
       </c>
       <c r="Z30">
         <v>29</v>
       </c>
       <c r="AA30">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="AB30">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="AB30">
-        <f t="shared" si="1"/>
-        <v>0.82758620689655171</v>
+        <v>0.7931034482758621</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
@@ -7362,12 +7362,12 @@
         <v>30</v>
       </c>
       <c r="AA31">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="AB31">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="AB31">
-        <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
@@ -7402,7 +7402,7 @@
         <v>15</v>
       </c>
       <c r="S32" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U32" t="s">
         <v>1761</v>
@@ -7411,12 +7411,12 @@
         <v>31</v>
       </c>
       <c r="AA32">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="AB32">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="AB32">
-        <f t="shared" si="1"/>
-        <v>0.83870967741935487</v>
+        <v>0.80645161290322576</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
@@ -7451,18 +7451,18 @@
         <v>778</v>
       </c>
       <c r="S33" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Z33">
         <v>32</v>
       </c>
       <c r="AA33">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="AB33">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="AB33">
-        <f t="shared" si="1"/>
-        <v>0.84375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
@@ -7497,7 +7497,7 @@
         <v>62</v>
       </c>
       <c r="S34" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U34" t="s">
         <v>719</v>
@@ -7506,12 +7506,12 @@
         <v>33</v>
       </c>
       <c r="AA34">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="AB34">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="AB34">
-        <f t="shared" si="1"/>
-        <v>0.84848484848484851</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
@@ -7545,19 +7545,19 @@
       <c r="Q35" t="s">
         <v>66</v>
       </c>
-      <c r="S35" s="5" t="s">
-        <v>716</v>
+      <c r="S35" s="5">
+        <v>-2</v>
       </c>
       <c r="Z35">
         <v>34</v>
       </c>
       <c r="AA35">
-        <f t="shared" ref="AA35:AA66" si="2">AA34+(IF(ISNUMBER(S35),1,0))</f>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="1"/>
-        <v>0.82352941176470584</v>
+        <f t="shared" si="0"/>
+        <v>0.79411764705882348</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.3">
@@ -7591,8 +7591,8 @@
       <c r="Q36" t="s">
         <v>68</v>
       </c>
-      <c r="S36" s="3" t="s">
-        <v>715</v>
+      <c r="S36" s="3">
+        <v>-2</v>
       </c>
       <c r="U36" t="s">
         <v>803</v>
@@ -7601,12 +7601,12 @@
         <v>35</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.77142857142857146</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
@@ -7640,8 +7640,8 @@
       <c r="Q37" t="s">
         <v>71</v>
       </c>
-      <c r="S37" s="3" t="s">
-        <v>715</v>
+      <c r="S37" s="3">
+        <v>-2</v>
       </c>
       <c r="U37" t="s">
         <v>804</v>
@@ -7650,12 +7650,12 @@
         <v>36</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="1"/>
-        <v>0.77777777777777779</v>
+        <f t="shared" si="0"/>
+        <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
@@ -7690,18 +7690,18 @@
         <v>780</v>
       </c>
       <c r="S38" s="1">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="Z38">
         <v>37</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="1"/>
-        <v>0.78378378378378377</v>
+        <f t="shared" si="0"/>
+        <v>0.72972972972972971</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
@@ -7735,8 +7735,8 @@
       <c r="Q39" t="s">
         <v>74</v>
       </c>
-      <c r="S39" s="5" t="s">
-        <v>716</v>
+      <c r="S39" s="5">
+        <v>7</v>
       </c>
       <c r="U39" t="s">
         <v>805</v>
@@ -7745,12 +7745,12 @@
         <v>38</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="1"/>
-        <v>0.76315789473684215</v>
+        <f t="shared" si="0"/>
+        <v>0.73684210526315785</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
@@ -7784,8 +7784,8 @@
       <c r="Q40" t="s">
         <v>782</v>
       </c>
-      <c r="S40" s="2" t="s">
-        <v>715</v>
+      <c r="S40" s="2">
+        <v>-1</v>
       </c>
       <c r="U40" t="s">
         <v>850</v>
@@ -7794,12 +7794,12 @@
         <v>39</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="1"/>
-        <v>0.74358974358974361</v>
+        <f t="shared" si="0"/>
+        <v>0.71794871794871795</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
@@ -7834,18 +7834,18 @@
         <v>77</v>
       </c>
       <c r="S41" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z41">
         <v>40</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
@@ -7879,8 +7879,8 @@
       <c r="Q42" t="s">
         <v>80</v>
       </c>
-      <c r="S42" s="5" t="s">
-        <v>716</v>
+      <c r="S42" s="5">
+        <v>-2</v>
       </c>
       <c r="U42" t="s">
         <v>851</v>
@@ -7889,12 +7889,12 @@
         <v>41</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="1"/>
-        <v>0.73170731707317072</v>
+        <f t="shared" si="0"/>
+        <v>0.70731707317073167</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
@@ -7929,18 +7929,18 @@
         <v>82</v>
       </c>
       <c r="S43" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Z43">
         <v>42</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="2"/>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="1"/>
-        <v>0.73809523809523814</v>
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
@@ -7975,18 +7975,18 @@
         <v>84</v>
       </c>
       <c r="S44" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z44">
         <v>43</v>
       </c>
       <c r="AA44">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="1"/>
-        <v>0.7441860465116279</v>
+        <f t="shared" si="0"/>
+        <v>0.72093023255813948</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
@@ -8021,7 +8021,7 @@
         <v>86</v>
       </c>
       <c r="S45" s="1">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="T45" s="2"/>
       <c r="U45" t="s">
@@ -8031,12 +8031,12 @@
         <v>44</v>
       </c>
       <c r="AA45">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0.70454545454545459</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
@@ -8070,8 +8070,8 @@
       <c r="Q46" t="s">
         <v>88</v>
       </c>
-      <c r="S46" s="5" t="s">
-        <v>716</v>
+      <c r="S46" s="5">
+        <v>7</v>
       </c>
       <c r="U46" t="s">
         <v>853</v>
@@ -8080,12 +8080,12 @@
         <v>45</v>
       </c>
       <c r="AA46">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="1"/>
-        <v>0.73333333333333328</v>
+        <f t="shared" si="0"/>
+        <v>0.71111111111111114</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
@@ -8120,19 +8120,19 @@
         <v>91</v>
       </c>
       <c r="S47" s="1">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="T47" s="2"/>
       <c r="Z47">
         <v>46</v>
       </c>
       <c r="AA47">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="AB47">
-        <f t="shared" si="1"/>
-        <v>0.73913043478260865</v>
+        <f t="shared" si="0"/>
+        <v>0.69565217391304346</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
@@ -8166,8 +8166,8 @@
       <c r="Q48" t="s">
         <v>93</v>
       </c>
-      <c r="S48" s="3" t="s">
-        <v>715</v>
+      <c r="S48" s="3">
+        <v>7</v>
       </c>
       <c r="U48" t="s">
         <v>854</v>
@@ -8176,12 +8176,12 @@
         <v>47</v>
       </c>
       <c r="AA48">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="1"/>
-        <v>0.72340425531914898</v>
+        <f t="shared" si="0"/>
+        <v>0.7021276595744681</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.3">
@@ -8216,7 +8216,7 @@
         <v>59</v>
       </c>
       <c r="S49" s="1">
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="U49" t="s">
         <v>857</v>
@@ -8225,12 +8225,12 @@
         <v>48</v>
       </c>
       <c r="AA49">
-        <f t="shared" si="2"/>
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB49">
-        <f t="shared" si="1"/>
-        <v>0.72916666666666663</v>
+        <f t="shared" si="0"/>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.3">
@@ -8265,7 +8265,7 @@
         <v>59</v>
       </c>
       <c r="S50" s="4">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="U50" t="s">
         <v>855</v>
@@ -8274,12 +8274,12 @@
         <v>49</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="1"/>
-        <v>0.73469387755102045</v>
+        <f t="shared" si="0"/>
+        <v>0.67346938775510201</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.3">
@@ -8313,8 +8313,8 @@
       <c r="Q51" t="s">
         <v>97</v>
       </c>
-      <c r="S51" s="3" t="s">
-        <v>715</v>
+      <c r="S51" s="3">
+        <v>-2</v>
       </c>
       <c r="U51" t="s">
         <v>1801</v>
@@ -8323,12 +8323,12 @@
         <v>50</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
+        <f t="shared" si="0"/>
+        <v>0.66</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.3">
@@ -8363,7 +8363,7 @@
         <v>246</v>
       </c>
       <c r="S52" s="1">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="U52" t="s">
         <v>858</v>
@@ -8372,12 +8372,12 @@
         <v>51</v>
       </c>
       <c r="AA52">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="1"/>
-        <v>0.72549019607843135</v>
+        <f t="shared" si="0"/>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.3">
@@ -8411,8 +8411,8 @@
       <c r="Q53" t="s">
         <v>99</v>
       </c>
-      <c r="S53" s="3" t="s">
-        <v>715</v>
+      <c r="S53" s="3">
+        <v>-2</v>
       </c>
       <c r="U53" t="s">
         <v>859</v>
@@ -8421,12 +8421,12 @@
         <v>52</v>
       </c>
       <c r="AA53">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="1"/>
-        <v>0.71153846153846156</v>
+        <f t="shared" si="0"/>
+        <v>0.63461538461538458</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.3">
@@ -8460,8 +8460,8 @@
       <c r="Q54" t="s">
         <v>101</v>
       </c>
-      <c r="S54" s="3" t="s">
-        <v>715</v>
+      <c r="S54" s="3">
+        <v>6</v>
       </c>
       <c r="U54" t="s">
         <v>860</v>
@@ -8470,12 +8470,12 @@
         <v>53</v>
       </c>
       <c r="AA54">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="1"/>
-        <v>0.69811320754716977</v>
+        <f t="shared" si="0"/>
+        <v>0.64150943396226412</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.3">
@@ -8509,8 +8509,8 @@
       <c r="Q55" t="s">
         <v>32</v>
       </c>
-      <c r="S55" s="5" t="s">
-        <v>716</v>
+      <c r="S55" s="5">
+        <v>-1</v>
       </c>
       <c r="T55" s="2"/>
       <c r="U55" t="s">
@@ -8520,12 +8520,12 @@
         <v>54</v>
       </c>
       <c r="AA55">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AB55">
-        <f t="shared" si="1"/>
-        <v>0.68518518518518523</v>
+        <f t="shared" si="0"/>
+        <v>0.62962962962962965</v>
       </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.3">
@@ -8559,8 +8559,8 @@
       <c r="Q56" t="s">
         <v>27</v>
       </c>
-      <c r="S56" s="3" t="s">
-        <v>715</v>
+      <c r="S56" s="3">
+        <v>-1</v>
       </c>
       <c r="T56" s="5"/>
       <c r="U56" t="s">
@@ -8570,12 +8570,12 @@
         <v>55</v>
       </c>
       <c r="AA56">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AB56">
-        <f t="shared" si="1"/>
-        <v>0.67272727272727273</v>
+        <f t="shared" si="0"/>
+        <v>0.61818181818181817</v>
       </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.3">
@@ -8610,7 +8610,7 @@
         <v>38</v>
       </c>
       <c r="S57" s="1">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="U57" t="s">
         <v>863</v>
@@ -8619,12 +8619,12 @@
         <v>56</v>
       </c>
       <c r="AA57">
-        <f t="shared" si="2"/>
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AB57">
-        <f t="shared" si="1"/>
-        <v>0.6785714285714286</v>
+        <f t="shared" si="0"/>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.3">
@@ -8659,7 +8659,7 @@
         <v>107</v>
       </c>
       <c r="S58" s="1">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="T58" s="3"/>
       <c r="U58" t="s">
@@ -8669,12 +8669,12 @@
         <v>57</v>
       </c>
       <c r="AA58">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AB58">
-        <f t="shared" si="1"/>
-        <v>0.68421052631578949</v>
+        <f t="shared" si="0"/>
+        <v>0.59649122807017541</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.3">
@@ -8708,8 +8708,8 @@
       <c r="Q59" t="s">
         <v>55</v>
       </c>
-      <c r="S59" s="3" t="s">
-        <v>715</v>
+      <c r="S59" s="3">
+        <v>7</v>
       </c>
       <c r="U59" t="s">
         <v>865</v>
@@ -8718,12 +8718,12 @@
         <v>58</v>
       </c>
       <c r="AA59">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="AB59">
-        <f t="shared" si="1"/>
-        <v>0.67241379310344829</v>
+        <f t="shared" si="0"/>
+        <v>0.60344827586206895</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.3">
@@ -8758,7 +8758,7 @@
         <v>53</v>
       </c>
       <c r="S60" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T60" s="3"/>
       <c r="U60" t="s">
@@ -8768,12 +8768,12 @@
         <v>59</v>
       </c>
       <c r="AA60">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="AB60">
-        <f t="shared" si="1"/>
-        <v>0.67796610169491522</v>
+        <f t="shared" si="0"/>
+        <v>0.59322033898305082</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.3">
@@ -8808,7 +8808,7 @@
         <v>19</v>
       </c>
       <c r="S61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U61" t="s">
         <v>1578</v>
@@ -8817,12 +8817,12 @@
         <v>60</v>
       </c>
       <c r="AA61">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="AB61">
-        <f t="shared" si="1"/>
-        <v>0.68333333333333335</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.3">
@@ -8856,8 +8856,8 @@
       <c r="Q62" t="s">
         <v>112</v>
       </c>
-      <c r="S62" s="5" t="s">
-        <v>716</v>
+      <c r="S62" s="5">
+        <v>6</v>
       </c>
       <c r="U62" t="s">
         <v>867</v>
@@ -8866,12 +8866,12 @@
         <v>61</v>
       </c>
       <c r="AA62">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
       <c r="AB62">
-        <f t="shared" si="1"/>
-        <v>0.67213114754098358</v>
+        <f t="shared" si="0"/>
+        <v>0.60655737704918034</v>
       </c>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.3">
@@ -8905,19 +8905,19 @@
       <c r="Q63" t="s">
         <v>114</v>
       </c>
-      <c r="S63" s="5" t="s">
-        <v>716</v>
+      <c r="S63" s="5">
+        <v>6</v>
       </c>
       <c r="Z63">
         <v>62</v>
       </c>
       <c r="AA63">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="AB63">
-        <f t="shared" si="1"/>
-        <v>0.66129032258064513</v>
+        <f t="shared" si="0"/>
+        <v>0.61290322580645162</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.3">
@@ -8951,19 +8951,19 @@
       <c r="Q64" t="s">
         <v>117</v>
       </c>
-      <c r="S64" s="3" t="s">
-        <v>715</v>
+      <c r="S64" s="3">
+        <v>-2</v>
       </c>
       <c r="Z64">
         <v>63</v>
       </c>
       <c r="AA64">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="AB64">
-        <f t="shared" si="1"/>
-        <v>0.65079365079365081</v>
+        <f t="shared" si="0"/>
+        <v>0.60317460317460314</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.3">
@@ -8997,8 +8997,8 @@
       <c r="Q65" t="s">
         <v>119</v>
       </c>
-      <c r="S65" s="2" t="s">
-        <v>716</v>
+      <c r="S65" s="2">
+        <v>-1</v>
       </c>
       <c r="T65" s="1">
         <v>7</v>
@@ -9010,12 +9010,12 @@
         <v>64</v>
       </c>
       <c r="AA65">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="AB65">
-        <f t="shared" si="1"/>
-        <v>0.640625</v>
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.3">
@@ -9049,8 +9049,8 @@
       <c r="Q66" t="s">
         <v>97</v>
       </c>
-      <c r="S66" s="3" t="s">
-        <v>715</v>
+      <c r="S66" s="3">
+        <v>-1</v>
       </c>
       <c r="U66" t="s">
         <v>804</v>
@@ -9059,12 +9059,12 @@
         <v>65</v>
       </c>
       <c r="AA66">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="AB66">
-        <f t="shared" si="1"/>
-        <v>0.63076923076923075</v>
+        <f t="shared" si="0"/>
+        <v>0.58461538461538465</v>
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.3">
@@ -9098,8 +9098,8 @@
       <c r="Q67" t="s">
         <v>86</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>716</v>
+      <c r="S67" s="5">
+        <v>7</v>
       </c>
       <c r="U67" t="s">
         <v>869</v>
@@ -9108,12 +9108,12 @@
         <v>66</v>
       </c>
       <c r="AA67">
-        <f t="shared" ref="AA67:AA101" si="3">AA66+(IF(ISNUMBER(S67),1,0))</f>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="AB67">
-        <f t="shared" ref="AB67:AB101" si="4">AA67/Z67</f>
-        <v>0.62121212121212122</v>
+        <f t="shared" ref="AB67:AB101" si="2">AA67/Z67</f>
+        <v>0.59090909090909094</v>
       </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.3">
@@ -9147,19 +9147,19 @@
       <c r="Q68" t="s">
         <v>127</v>
       </c>
-      <c r="S68" s="5" t="s">
-        <v>716</v>
+      <c r="S68" s="5">
+        <v>-1</v>
       </c>
       <c r="Z68">
         <v>67</v>
       </c>
       <c r="AA68">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="AB68">
-        <f t="shared" si="4"/>
-        <v>0.61194029850746268</v>
+        <f t="shared" si="2"/>
+        <v>0.58208955223880599</v>
       </c>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.3">
@@ -9193,8 +9193,8 @@
       <c r="Q69" t="s">
         <v>131</v>
       </c>
-      <c r="S69" s="5" t="s">
-        <v>716</v>
+      <c r="S69" s="5">
+        <v>-1</v>
       </c>
       <c r="T69" s="6"/>
       <c r="U69" t="s">
@@ -9204,12 +9204,12 @@
         <v>68</v>
       </c>
       <c r="AA69">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <f t="shared" ref="AA69:AA101" si="3">AA68+IF(S69 &gt; 0,1,0)</f>
+        <v>39</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="4"/>
-        <v>0.6029411764705882</v>
+        <f t="shared" si="2"/>
+        <v>0.57352941176470584</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.3">
@@ -9243,19 +9243,19 @@
       <c r="Q70" t="s">
         <v>38</v>
       </c>
-      <c r="S70" s="5" t="s">
-        <v>716</v>
+      <c r="S70" s="5">
+        <v>7</v>
       </c>
       <c r="Z70">
         <v>69</v>
       </c>
       <c r="AA70">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="4"/>
-        <v>0.59420289855072461</v>
+        <f t="shared" si="2"/>
+        <v>0.57971014492753625</v>
       </c>
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.3">
@@ -9289,8 +9289,8 @@
       <c r="Q71" t="s">
         <v>135</v>
       </c>
-      <c r="S71" s="5" t="s">
-        <v>716</v>
+      <c r="S71" s="5">
+        <v>7</v>
       </c>
       <c r="T71" s="6"/>
       <c r="U71" t="s">
@@ -9304,7 +9304,7 @@
         <v>41</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.58571428571428574</v>
       </c>
     </row>
@@ -9339,8 +9339,8 @@
       <c r="Q72" t="s">
         <v>137</v>
       </c>
-      <c r="S72" s="5" t="s">
-        <v>716</v>
+      <c r="S72" s="5">
+        <v>-2</v>
       </c>
       <c r="Z72">
         <v>71</v>
@@ -9350,7 +9350,7 @@
         <v>41</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.57746478873239437</v>
       </c>
     </row>
@@ -9385,8 +9385,8 @@
       <c r="Q73" t="s">
         <v>139</v>
       </c>
-      <c r="S73" s="5" t="s">
-        <v>716</v>
+      <c r="S73" s="5">
+        <v>-2</v>
       </c>
       <c r="Z73">
         <v>72</v>
@@ -9396,7 +9396,7 @@
         <v>41</v>
       </c>
       <c r="AB73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.56944444444444442</v>
       </c>
     </row>
@@ -9431,8 +9431,8 @@
       <c r="Q74" t="s">
         <v>142</v>
       </c>
-      <c r="S74" s="5" t="s">
-        <v>716</v>
+      <c r="S74" s="5">
+        <v>-1</v>
       </c>
       <c r="Z74">
         <v>73</v>
@@ -9442,7 +9442,7 @@
         <v>41</v>
       </c>
       <c r="AB74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.56164383561643838</v>
       </c>
     </row>
@@ -9478,7 +9478,7 @@
         <v>840</v>
       </c>
       <c r="S75" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U75" t="s">
         <v>877</v>
@@ -9491,7 +9491,7 @@
         <v>42</v>
       </c>
       <c r="AB75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.56756756756756754</v>
       </c>
     </row>
@@ -9526,8 +9526,8 @@
       <c r="Q76" t="s">
         <v>144</v>
       </c>
-      <c r="S76" s="5" t="s">
-        <v>716</v>
+      <c r="S76" s="5">
+        <v>7</v>
       </c>
       <c r="T76" s="6"/>
       <c r="U76" t="s">
@@ -9538,11 +9538,11 @@
       </c>
       <c r="AA76">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB76">
-        <f t="shared" si="4"/>
-        <v>0.56000000000000005</v>
+        <f t="shared" si="2"/>
+        <v>0.57333333333333336</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.3">
@@ -9577,7 +9577,7 @@
         <v>59</v>
       </c>
       <c r="S77" s="4">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="U77" t="s">
         <v>856</v>
@@ -9590,7 +9590,7 @@
         <v>43</v>
       </c>
       <c r="AB77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.56578947368421051</v>
       </c>
     </row>
@@ -9625,19 +9625,19 @@
       <c r="Q78" t="s">
         <v>785</v>
       </c>
-      <c r="S78" s="5" t="s">
-        <v>716</v>
+      <c r="S78" s="5">
+        <v>11</v>
       </c>
       <c r="Z78">
         <v>77</v>
       </c>
       <c r="AA78">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AB78">
-        <f t="shared" si="4"/>
-        <v>0.55844155844155841</v>
+        <f t="shared" si="2"/>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.3">
@@ -9671,19 +9671,19 @@
       <c r="Q79" t="s">
         <v>129</v>
       </c>
-      <c r="S79" s="5" t="s">
-        <v>716</v>
+      <c r="S79" s="5">
+        <v>7</v>
       </c>
       <c r="Z79">
         <v>78</v>
       </c>
       <c r="AA79">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AB79">
-        <f t="shared" si="4"/>
-        <v>0.55128205128205132</v>
+        <f t="shared" si="2"/>
+        <v>0.57692307692307687</v>
       </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.3">
@@ -9718,18 +9718,18 @@
         <v>148</v>
       </c>
       <c r="S80" s="1">
-        <v>11</v>
+        <v>-2</v>
       </c>
       <c r="Z80">
         <v>79</v>
       </c>
       <c r="AA80">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB80">
-        <f t="shared" si="4"/>
-        <v>0.55696202531645567</v>
+        <f t="shared" si="2"/>
+        <v>0.569620253164557</v>
       </c>
     </row>
     <row r="81" spans="1:28" x14ac:dyDescent="0.3">
@@ -9763,19 +9763,19 @@
       <c r="Q81" t="s">
         <v>150</v>
       </c>
-      <c r="S81" s="5" t="s">
-        <v>716</v>
+      <c r="S81" s="5">
+        <v>-2</v>
       </c>
       <c r="Z81">
         <v>80</v>
       </c>
       <c r="AA81">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB81">
-        <f t="shared" si="4"/>
-        <v>0.55000000000000004</v>
+        <f t="shared" si="2"/>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.3">
@@ -9809,8 +9809,8 @@
       <c r="Q82" t="s">
         <v>786</v>
       </c>
-      <c r="S82" s="5" t="s">
-        <v>716</v>
+      <c r="S82" s="5">
+        <v>-2</v>
       </c>
       <c r="T82" s="6"/>
       <c r="Z82">
@@ -9818,11 +9818,11 @@
       </c>
       <c r="AA82">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB82">
-        <f t="shared" si="4"/>
-        <v>0.54320987654320985</v>
+        <f t="shared" si="2"/>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.3">
@@ -9856,8 +9856,8 @@
       <c r="Q83" t="s">
         <v>152</v>
       </c>
-      <c r="S83" s="3" t="s">
-        <v>715</v>
+      <c r="S83" s="3">
+        <v>-2</v>
       </c>
       <c r="T83" s="1">
         <v>3</v>
@@ -9870,11 +9870,11 @@
       </c>
       <c r="AA83">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB83">
-        <f t="shared" si="4"/>
-        <v>0.53658536585365857</v>
+        <f t="shared" si="2"/>
+        <v>0.54878048780487809</v>
       </c>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.3">
@@ -9908,8 +9908,8 @@
       <c r="Q84" t="s">
         <v>155</v>
       </c>
-      <c r="S84" s="5" t="s">
-        <v>716</v>
+      <c r="S84" s="5">
+        <v>-2</v>
       </c>
       <c r="U84" t="s">
         <v>1767</v>
@@ -9919,11 +9919,11 @@
       </c>
       <c r="AA84">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB84">
-        <f t="shared" si="4"/>
-        <v>0.53012048192771088</v>
+        <f t="shared" si="2"/>
+        <v>0.54216867469879515</v>
       </c>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.3">
@@ -9957,19 +9957,19 @@
       <c r="Q85" t="s">
         <v>157</v>
       </c>
-      <c r="S85" s="5" t="s">
-        <v>716</v>
+      <c r="S85" s="5">
+        <v>-2</v>
       </c>
       <c r="Z85">
         <v>84</v>
       </c>
       <c r="AA85">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB85">
-        <f t="shared" si="4"/>
-        <v>0.52380952380952384</v>
+        <f t="shared" si="2"/>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.3">
@@ -10003,8 +10003,8 @@
       <c r="Q86" t="s">
         <v>159</v>
       </c>
-      <c r="S86" s="5" t="s">
-        <v>716</v>
+      <c r="S86" s="5">
+        <v>-2</v>
       </c>
       <c r="U86" t="s">
         <v>1768</v>
@@ -10014,11 +10014,11 @@
       </c>
       <c r="AA86">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB86">
-        <f t="shared" si="4"/>
-        <v>0.51764705882352946</v>
+        <f t="shared" si="2"/>
+        <v>0.52941176470588236</v>
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.3">
@@ -10053,7 +10053,7 @@
         <v>161</v>
       </c>
       <c r="S87" s="1">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="U87" t="s">
         <v>1769</v>
@@ -10066,7 +10066,7 @@
         <v>45</v>
       </c>
       <c r="AB87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.52325581395348841</v>
       </c>
     </row>
@@ -10101,8 +10101,8 @@
       <c r="Q88" t="s">
         <v>164</v>
       </c>
-      <c r="S88" s="3" t="s">
-        <v>715</v>
+      <c r="S88" s="3">
+        <v>-2</v>
       </c>
       <c r="U88" t="s">
         <v>1768</v>
@@ -10115,7 +10115,7 @@
         <v>45</v>
       </c>
       <c r="AB88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.51724137931034486</v>
       </c>
     </row>
@@ -10151,7 +10151,7 @@
         <v>166</v>
       </c>
       <c r="S89" s="1">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="T89" s="7"/>
       <c r="Z89">
@@ -10159,11 +10159,11 @@
       </c>
       <c r="AA89">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB89">
-        <f t="shared" si="4"/>
-        <v>0.52272727272727271</v>
+        <f t="shared" si="2"/>
+        <v>0.51136363636363635</v>
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.3">
@@ -10197,19 +10197,19 @@
       <c r="Q90" t="s">
         <v>82</v>
       </c>
-      <c r="S90" s="5" t="s">
-        <v>716</v>
+      <c r="S90" s="5">
+        <v>-2</v>
       </c>
       <c r="Z90">
         <v>89</v>
       </c>
       <c r="AA90">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB90">
-        <f t="shared" si="4"/>
-        <v>0.5168539325842697</v>
+        <f t="shared" si="2"/>
+        <v>0.5056179775280899</v>
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.3">
@@ -10243,19 +10243,19 @@
       <c r="Q91" t="s">
         <v>169</v>
       </c>
-      <c r="S91" s="5" t="s">
-        <v>716</v>
+      <c r="S91" s="5">
+        <v>-2</v>
       </c>
       <c r="Z91">
         <v>90</v>
       </c>
       <c r="AA91">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB91">
-        <f t="shared" si="4"/>
-        <v>0.51111111111111107</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.3">
@@ -10290,18 +10290,18 @@
         <v>171</v>
       </c>
       <c r="S92" s="1">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="Z92">
         <v>91</v>
       </c>
       <c r="AA92">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AB92">
-        <f t="shared" si="4"/>
-        <v>0.51648351648351654</v>
+        <f t="shared" si="2"/>
+        <v>0.49450549450549453</v>
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.3">
@@ -10335,19 +10335,19 @@
       <c r="Q93" t="s">
         <v>706</v>
       </c>
-      <c r="S93" s="5" t="s">
-        <v>716</v>
+      <c r="S93" s="5">
+        <v>-2</v>
       </c>
       <c r="Z93">
         <v>92</v>
       </c>
       <c r="AA93">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AB93">
-        <f t="shared" si="4"/>
-        <v>0.51086956521739135</v>
+        <f t="shared" si="2"/>
+        <v>0.4891304347826087</v>
       </c>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.3">
@@ -10382,7 +10382,7 @@
         <v>787</v>
       </c>
       <c r="S94" s="1">
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="U94" t="s">
         <v>1770</v>
@@ -10392,11 +10392,11 @@
       </c>
       <c r="AA94">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB94">
-        <f t="shared" si="4"/>
-        <v>0.5161290322580645</v>
+        <f t="shared" si="2"/>
+        <v>0.4838709677419355</v>
       </c>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.3">
@@ -10430,19 +10430,19 @@
       <c r="Q95" t="s">
         <v>173</v>
       </c>
-      <c r="S95" s="5" t="s">
-        <v>716</v>
+      <c r="S95" s="5">
+        <v>-2</v>
       </c>
       <c r="Z95">
         <v>94</v>
       </c>
       <c r="AA95">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB95">
-        <f t="shared" si="4"/>
-        <v>0.51063829787234039</v>
+        <f t="shared" si="2"/>
+        <v>0.47872340425531917</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.3">
@@ -10476,8 +10476,8 @@
       <c r="Q96" t="s">
         <v>131</v>
       </c>
-      <c r="S96" s="5" t="s">
-        <v>716</v>
+      <c r="S96" s="5">
+        <v>-2</v>
       </c>
       <c r="U96" t="s">
         <v>1767</v>
@@ -10487,11 +10487,11 @@
       </c>
       <c r="AA96">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB96">
-        <f t="shared" si="4"/>
-        <v>0.50526315789473686</v>
+        <f t="shared" si="2"/>
+        <v>0.47368421052631576</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.3">
@@ -10525,19 +10525,19 @@
       <c r="Q97" t="s">
         <v>176</v>
       </c>
-      <c r="S97" s="5" t="s">
-        <v>716</v>
+      <c r="S97" s="5">
+        <v>-2</v>
       </c>
       <c r="Z97">
         <v>96</v>
       </c>
       <c r="AA97">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB97">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.3">
@@ -10571,19 +10571,19 @@
       <c r="Q98" t="s">
         <v>73</v>
       </c>
-      <c r="S98" s="5" t="s">
-        <v>716</v>
+      <c r="S98" s="5">
+        <v>-2</v>
       </c>
       <c r="Z98">
         <v>97</v>
       </c>
       <c r="AA98">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB98">
-        <f t="shared" si="4"/>
-        <v>0.49484536082474229</v>
+        <f t="shared" si="2"/>
+        <v>0.46391752577319589</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.3">
@@ -10617,8 +10617,8 @@
       <c r="Q99" t="s">
         <v>181</v>
       </c>
-      <c r="S99" s="5" t="s">
-        <v>716</v>
+      <c r="S99" s="5">
+        <v>-2</v>
       </c>
       <c r="U99" t="s">
         <v>1768</v>
@@ -10628,11 +10628,11 @@
       </c>
       <c r="AA99">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB99">
-        <f t="shared" si="4"/>
-        <v>0.48979591836734693</v>
+        <f t="shared" si="2"/>
+        <v>0.45918367346938777</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.3">
@@ -10667,18 +10667,18 @@
         <v>183</v>
       </c>
       <c r="S100" s="1">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="Z100">
         <v>99</v>
       </c>
       <c r="AA100">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AB100">
-        <f t="shared" si="4"/>
-        <v>0.49494949494949497</v>
+        <f t="shared" si="2"/>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.3">
@@ -10712,19 +10712,19 @@
       <c r="Q101" t="s">
         <v>186</v>
       </c>
-      <c r="S101" s="5" t="s">
-        <v>716</v>
+      <c r="S101" s="5">
+        <v>-1</v>
       </c>
       <c r="Z101">
         <v>100</v>
       </c>
       <c r="AA101">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AB101">
-        <f t="shared" si="4"/>
-        <v>0.49</v>
+        <f t="shared" si="2"/>
+        <v>0.45</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.3">

</xml_diff>